<commit_message>
Uploading on git repository
</commit_message>
<xml_diff>
--- a/wordsInHindi/newtempwordsInHindi.xlsx
+++ b/wordsInHindi/newtempwordsInHindi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pramil\Desktop\programming\HTML\wordsInHindi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pramil\Desktop\programming\HTML\HindiProject\wordsInHindi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DB9232-B79D-4073-BD06-1BEAE79AA7B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA64B6B-6095-4D83-BB60-30B5EBE10EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{91C3D72C-7987-4B7C-8532-4C41DA595132}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>किताब</t>
   </si>
@@ -71,48 +71,12 @@
     <t xml:space="preserve">sound </t>
   </si>
   <si>
-    <t>endSound</t>
-  </si>
-  <si>
-    <t>begSound</t>
-  </si>
-  <si>
-    <t>possibeWords</t>
-  </si>
-  <si>
-    <t>क</t>
-  </si>
-  <si>
-    <t>ब</t>
-  </si>
-  <si>
-    <t>प</t>
-  </si>
-  <si>
-    <t>र</t>
-  </si>
-  <si>
-    <t>किताब खिताब कइताब कइतआब</t>
-  </si>
-  <si>
-    <t>परइवार परिबार परिवार परिवआर</t>
-  </si>
-  <si>
     <t>साइकिल</t>
   </si>
   <si>
     <t>स आ सा इ कि क इ ल</t>
   </si>
   <si>
-    <t>स</t>
-  </si>
-  <si>
-    <t>ल</t>
-  </si>
-  <si>
-    <t xml:space="preserve">सआइकल साइकिल साइकइल </t>
-  </si>
-  <si>
     <t>गिटार</t>
   </si>
   <si>
@@ -158,39 +122,6 @@
     <t>ग उ गु ल आ ला ब ई बी</t>
   </si>
   <si>
-    <t>ग</t>
-  </si>
-  <si>
-    <t>त</t>
-  </si>
-  <si>
-    <t>म</t>
-  </si>
-  <si>
-    <t>द</t>
-  </si>
-  <si>
-    <t>न</t>
-  </si>
-  <si>
-    <t>गिटार घिटार गिठार घिठार</t>
-  </si>
-  <si>
-    <t>तितली टिटली तइतली टइटली</t>
-  </si>
-  <si>
-    <t>लढ़की लड़की लड़कई लढ़कई</t>
-  </si>
-  <si>
-    <t>मचलई मचली मछलई मछली</t>
-  </si>
-  <si>
-    <t>डुकान दुकान डउकान दउकान</t>
-  </si>
-  <si>
-    <t>गउलाबी गुलाबी घउलाबी घुलाबी</t>
-  </si>
-  <si>
     <t>picbutterfly.jpg</t>
   </si>
   <si>
@@ -218,10 +149,31 @@
     <t>च छ ई ची छी त ट आ ता</t>
   </si>
   <si>
-    <t>च</t>
-  </si>
-  <si>
-    <t xml:space="preserve">चीता छीता चीटा छीटा </t>
+    <t>status</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>soundfish.mp4</t>
+  </si>
+  <si>
+    <t>soundgirl.mp4</t>
+  </si>
+  <si>
+    <t>soundPariwar.mp4</t>
+  </si>
+  <si>
+    <t>soundtitli.mp4</t>
+  </si>
+  <si>
+    <t>soundGuitar.mp4</t>
+  </si>
+  <si>
+    <t>soundDukan.mp4</t>
   </si>
 </sst>
 </file>
@@ -579,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9B1D83-BE8B-474B-BDDD-5904D6967821}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -596,7 +548,7 @@
     <col min="8" max="8" width="39.9453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -613,16 +565,10 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -630,7 +576,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -639,16 +585,10 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -659,30 +599,24 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -691,102 +625,78 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>37</v>
-      </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -795,91 +705,67 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
-      </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>